<commit_message>
script to cleaning the dataset
</commit_message>
<xml_diff>
--- a/data/dictionary/Dicionário dos dados.xlsx
+++ b/data/dictionary/Dicionário dos dados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="290">
   <si>
     <t xml:space="preserve">Campos</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t xml:space="preserve">PH do solo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.0 para 2.80</t>
   </si>
   <si>
     <t xml:space="preserve">Mo</t>
@@ -1076,13 +1079,13 @@
   </sheetPr>
   <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C190" activeCellId="0" sqref="C190"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
@@ -1369,10 +1372,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1435,1332 +1438,1335 @@
       <c r="B44" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C44" s="0" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>